<commit_message>
added all files in data directory to output
</commit_message>
<xml_diff>
--- a/AssetTrackingApplication/Data/AssetTrackingTableNew.xlsx
+++ b/AssetTrackingApplication/Data/AssetTrackingTableNew.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AssetTracking\GitHub\AssetTrackingApplication\AssetTrackingApplication\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190DCC73-3CF3-4DED-95CD-76FAC92AC696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBEBE65-87B3-4889-9398-EFB55FC67B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D391F12-46A1-4978-9D89-E54DFF536296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -168,123 +164,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2">
-            <v>20607.693480000002</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>8553.5746500000005</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>29161.268130000004</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>101.47</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>0.02</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>8477.7699999999986</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>3917.3842296908001</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>5705.9495647288004</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>83.845449520000003</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>50.524214399999998</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>190.48915483168</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>89.828699503999999</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>11.820536000000001</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>70.245078767799995</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>29.400460800000001</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>10149.48738824308</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
added openfiledialog to choose file path for excel file
</commit_message>
<xml_diff>
--- a/AssetTrackingApplication/Data/AssetTrackingTableNew.xlsx
+++ b/AssetTrackingApplication/Data/AssetTrackingTableNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AssetTracking\GitHub\AssetTrackingApplication\AssetTrackingApplication\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBEBE65-87B3-4889-9398-EFB55FC67B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EE3CC5-732C-4377-904C-0616B3DB52CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D391F12-46A1-4978-9D89-E54DFF536296}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D391F12-46A1-4978-9D89-E54DFF536296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Asset</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Asset Class Total</t>
+  </si>
+  <si>
+    <t>Bank Accounts</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +155,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,12 +475,13 @@
   <dimension ref="A1:AQ150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
@@ -631,22 +641,48 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="4"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
+    <row r="8" spans="1:23" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <f>SUM(C2:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <f>SUM(D2:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <f>SUM(E2:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10" t="e">
+        <f>(C8-E8)/E8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="10" t="e">
+        <f>C8/D8-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="9">
+        <f>C8-D8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <f>SUM(K2:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="10"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
@@ -2887,31 +2923,31 @@
         <v>14</v>
       </c>
       <c r="B150" s="8"/>
-      <c r="C150" s="9" t="e">
-        <f>SUM(#REF!,C10,C30,C40,C50)</f>
-        <v>#REF!</v>
+      <c r="C150" s="9">
+        <f>SUM(C10,C30,C40,C50)</f>
+        <v>0</v>
       </c>
-      <c r="D150" s="9" t="e">
-        <f>SUM(#REF!,D10,D30,D40,D50)</f>
-        <v>#REF!</v>
+      <c r="D150" s="9">
+        <f>SUM(D10,D30,D40,D50)</f>
+        <v>0</v>
       </c>
-      <c r="E150" s="9" t="e">
-        <f>SUM(#REF!,E30,E40,E50)</f>
-        <v>#REF!</v>
+      <c r="E150" s="9">
+        <f>SUM(E10,E30,E40,E50)</f>
+        <v>0</v>
       </c>
       <c r="F150" s="9"/>
       <c r="G150" s="9"/>
       <c r="H150" s="10" t="e">
         <f>(C150-C10)/E150-1</f>
-        <v>#REF!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I150" s="10" t="e">
         <f>C150/D150 - 1</f>
-        <v>#REF!</v>
+        <v>#DIV/0!</v>
       </c>
-      <c r="J150" s="9" t="e">
+      <c r="J150" s="9">
         <f>C150-D150</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="K150" s="10"/>
       <c r="L150" s="11"/>

</xml_diff>